<commit_message>
Updates to milestone, README and proposal
</commit_message>
<xml_diff>
--- a/Ottawa Traffic Collision- Project milestones agile.xlsx
+++ b/Ottawa Traffic Collision- Project milestones agile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c53935ccf6d93ce3/Documents/Data Bootcamp/Assignments/16. ^0 17 Project 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c53935ccf6d93ce3/Documents/Data Bootcamp/Assignments/16. ^0 17 Project 3/Project_3_Exploring_Ottawa-s_Urban_Dynamics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{C2A56CB0-5949-4E1C-909F-FC65D7466D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C092BB83-0B0E-458C-87F2-5B978B9C3087}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{C2A56CB0-5949-4E1C-909F-FC65D7466D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{924779F3-4DD7-417E-B6BB-6BC3BA66A828}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8650E19-A6E3-4B1B-AD4E-477EE979450A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B8650E19-A6E3-4B1B-AD4E-477EE979450A}"/>
   </bookViews>
   <sheets>
     <sheet name="Project milestones" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>GOAL IS 100/100</t>
   </si>
@@ -113,9 +113,6 @@
     <t xml:space="preserve">Create Repository </t>
   </si>
   <si>
-    <t>What is the overarching theme - 2 major points</t>
-  </si>
-  <si>
     <t xml:space="preserve">Analysis/ Data visualizations </t>
   </si>
   <si>
@@ -128,18 +125,9 @@
     <t xml:space="preserve">This will be added to presentation deck </t>
   </si>
   <si>
-    <t>Combination of Jupyter notebook</t>
-  </si>
-  <si>
-    <t>Combining all analysis into one jupyter notebook</t>
-  </si>
-  <si>
     <t>Presentation Deck - 5/6 pager</t>
   </si>
   <si>
-    <t>2 major points will determine the flow of the deck and the storyline</t>
-  </si>
-  <si>
     <t>Share presentation across all the members</t>
   </si>
   <si>
@@ -176,25 +164,13 @@
     <t>Advisor| Engineering background</t>
   </si>
   <si>
-    <t>Next week</t>
-  </si>
-  <si>
     <t>Project 3</t>
   </si>
   <si>
-    <t>Module 9 - Module 15 |</t>
-  </si>
-  <si>
     <t>Apr 17th [9:30 - 11:00PM Toronto time]   Thursday</t>
   </si>
   <si>
     <t>April 19th [6:30 - 9:30 PM Toronto time]   Saturday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Days and Plan for each day till April 19th </t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <t xml:space="preserve">Pandas/ Matplotlib/Numpy/Seaborn / API/Flask/Folium </t>
@@ -216,6 +192,21 @@
   </si>
   <si>
     <t>Data Cleaning &amp; Database</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Combination of codes</t>
+  </si>
+  <si>
+    <t>Combining all codes</t>
+  </si>
+  <si>
+    <t>Module 10 - Module 14 |</t>
+  </si>
+  <si>
+    <t>Submitting April 21st</t>
   </si>
 </sst>
 </file>
@@ -288,7 +279,7 @@
     <font>
       <strike/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,21 +287,22 @@
     <font>
       <strike/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <strike/>
       <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -366,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -407,12 +399,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -431,39 +417,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,7 +765,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -801,7 +785,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -831,13 +815,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -859,7 +843,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -875,23 +859,24 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>50</v>
+      <c r="B11" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G12" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H13" s="12"/>
@@ -927,35 +912,35 @@
       <c r="D15" s="12">
         <v>45757</v>
       </c>
-      <c r="E15" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="16"/>
+      <c r="E15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="16">
+        <v>45757</v>
+      </c>
       <c r="H15"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="25">
         <v>45755</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="25">
         <v>45755</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="32">
+      <c r="E16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="27">
         <v>45755</v>
       </c>
-      <c r="G16" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="G16" s="20"/>
       <c r="H16"/>
       <c r="I16"/>
     </row>
@@ -967,9 +952,15 @@
       <c r="C17" s="12">
         <v>45757</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="16"/>
+      <c r="D17" s="12">
+        <v>45757</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="16">
+        <v>45758</v>
+      </c>
       <c r="H17"/>
       <c r="I17"/>
     </row>
@@ -978,7 +969,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C18" s="12">
         <v>45757</v>
@@ -986,53 +977,73 @@
       <c r="D18" s="12">
         <v>45755</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="16"/>
+      <c r="E18" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H18"/>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="12">
         <v>45757</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="16"/>
+      <c r="D19" s="12">
+        <v>45761</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="16">
+        <v>45762</v>
+      </c>
       <c r="H19"/>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C20" s="12">
         <v>45759</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="16"/>
+      <c r="D20" s="12">
+        <v>45762</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="16">
+        <v>45766</v>
+      </c>
       <c r="H20"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:11" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="13">
         <v>45762</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="16"/>
+      <c r="D21" s="12">
+        <v>45762</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="16">
+        <v>45766</v>
+      </c>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
@@ -1041,54 +1052,62 @@
     </row>
     <row r="22" spans="1:11" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C22" s="13">
         <v>45762</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="17"/>
+      <c r="D22" s="12">
+        <v>45762</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="16">
+        <v>45766</v>
+      </c>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C23" s="13">
         <v>45763</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="17"/>
+      <c r="D23" s="12">
+        <v>45762</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="16">
+        <v>45766</v>
+      </c>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:11" s="4" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="36">
-        <v>45763</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="21"/>
+      <c r="A24" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="19"/>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
@@ -1096,17 +1115,23 @@
     </row>
     <row r="25" spans="1:11" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C25" s="13">
         <v>45764</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="17"/>
+      <c r="D25" s="13">
+        <v>45766</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="17">
+        <v>45768</v>
+      </c>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
@@ -1114,21 +1139,27 @@
     </row>
     <row r="26" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C26" s="13">
         <v>45764</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="17"/>
+      <c r="D26" s="13">
+        <v>45764</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="17">
+        <v>45768</v>
+      </c>
       <c r="G26"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="23"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
@@ -1137,43 +1168,49 @@
       <c r="C27" s="13">
         <v>45766</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="17"/>
+      <c r="D27" s="13">
+        <v>45768</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="17">
+        <v>45768</v>
+      </c>
       <c r="G27"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="23"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
-      <c r="F28" s="24"/>
+      <c r="F28" s="22"/>
       <c r="G28"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="27"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
-      <c r="J29" s="23"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J30" s="23"/>
+        <v>34</v>
+      </c>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>